<commit_message>
notas de la practica
</commit_message>
<xml_diff>
--- a/OYM/_DocumentosComunes/_POO.xlsx
+++ b/OYM/_DocumentosComunes/_POO.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Page 1'!$A$1:$O$1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Page 1'!$A$1:$G$93</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Page 1'!$A$1:$G$90</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -1143,11 +1143,11 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:O190"/>
+  <dimension ref="A1:O90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1461,12 +1461,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
       <c r="K8">
         <v>1</v>
       </c>
       <c r="N8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1563,12 +1566,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="N11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1631,12 +1637,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I13">
+        <v>10</v>
+      </c>
       <c r="K13">
         <v>1</v>
       </c>
       <c r="N13">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1699,12 +1708,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I15">
+        <v>10</v>
+      </c>
       <c r="K15">
         <v>1</v>
       </c>
       <c r="N15">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1733,12 +1745,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I16">
+        <v>10</v>
+      </c>
       <c r="K16">
         <v>1</v>
       </c>
       <c r="N16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1801,12 +1816,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I18">
+        <v>10</v>
+      </c>
       <c r="K18">
         <v>1</v>
       </c>
       <c r="N18">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1869,12 +1887,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I20">
+        <v>10</v>
+      </c>
       <c r="K20">
         <v>1</v>
       </c>
       <c r="N20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1903,12 +1924,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I21">
+        <v>10</v>
+      </c>
       <c r="K21">
         <v>1</v>
       </c>
       <c r="N21">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1937,12 +1961,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I22">
+        <v>10</v>
+      </c>
       <c r="K22">
         <v>1</v>
       </c>
       <c r="N22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1971,12 +1998,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I23">
+        <v>10</v>
+      </c>
       <c r="K23">
         <v>1</v>
       </c>
       <c r="N23">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2107,12 +2137,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I27">
+        <v>10</v>
+      </c>
       <c r="K27">
         <v>1</v>
       </c>
       <c r="N27">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2141,12 +2174,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I28">
+        <v>10</v>
+      </c>
       <c r="K28">
         <v>1</v>
       </c>
       <c r="N28">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2209,12 +2245,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I30">
+        <v>10</v>
+      </c>
       <c r="K30">
         <v>1</v>
       </c>
       <c r="N30">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2379,12 +2418,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I35">
+        <v>10</v>
+      </c>
       <c r="K35">
         <v>1</v>
       </c>
       <c r="N35">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2549,12 +2591,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I40">
+        <v>10</v>
+      </c>
       <c r="K40">
         <v>1</v>
       </c>
       <c r="N40">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2617,12 +2662,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I42">
+        <v>10</v>
+      </c>
       <c r="K42">
         <v>1</v>
       </c>
       <c r="N42">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2651,12 +2699,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I43">
+        <v>10</v>
+      </c>
       <c r="K43">
         <v>1</v>
       </c>
       <c r="N43">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2685,12 +2736,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I44">
+        <v>10</v>
+      </c>
       <c r="K44">
         <v>1</v>
       </c>
       <c r="N44">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2957,12 +3011,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I52">
+        <v>10</v>
+      </c>
       <c r="K52">
         <v>1</v>
       </c>
       <c r="N52">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3025,12 +3082,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I54">
+        <v>10</v>
+      </c>
       <c r="K54">
         <v>1</v>
       </c>
       <c r="N54">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3195,12 +3255,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I59">
+        <v>10</v>
+      </c>
       <c r="K59">
         <v>1</v>
       </c>
       <c r="N59">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3229,12 +3292,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I60">
+        <v>10</v>
+      </c>
       <c r="K60">
         <v>1</v>
       </c>
       <c r="N60">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3263,12 +3329,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I61">
+        <v>10</v>
+      </c>
       <c r="K61">
         <v>1</v>
       </c>
       <c r="N61">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3297,12 +3366,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I62">
+        <v>10</v>
+      </c>
       <c r="K62">
         <v>1</v>
       </c>
       <c r="N62">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3331,12 +3403,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I63">
+        <v>10</v>
+      </c>
       <c r="K63">
         <v>1</v>
       </c>
       <c r="N63">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3365,12 +3440,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I64">
+        <v>10</v>
+      </c>
       <c r="K64">
         <v>1</v>
       </c>
       <c r="N64">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3399,12 +3477,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
+      <c r="I65">
+        <v>10</v>
+      </c>
       <c r="K65">
         <v>1</v>
       </c>
       <c r="N65">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3452,26 +3533,26 @@
         <v>145</v>
       </c>
       <c r="D67" s="6" t="str">
-        <f t="shared" ref="D67:D130" si="5">IF((N67)&gt;=70,10,"")</f>
+        <f t="shared" ref="D67:D90" si="5">IF((N67)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E67" s="2" t="str">
-        <f t="shared" ref="E67:E130" si="6">IF((N67)&gt;=70,20,"")</f>
+        <f t="shared" ref="E67:E90" si="6">IF((N67)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F67" s="2" t="str">
-        <f t="shared" ref="F67:F130" si="7">IF((N67)&gt;=70,20,"")</f>
+        <f t="shared" ref="F67:F90" si="7">IF((N67)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G67" s="6" t="str">
-        <f t="shared" ref="G67:G118" si="8">IF((N67)&gt;=70,IF((N67-50)&gt;50,50,IF((N67-50)&lt;0,0,(N67-50))), "" )</f>
+        <f t="shared" ref="G67:G90" si="8">IF((N67)&gt;=70,IF((N67-50)&gt;50,50,IF((N67-50)&lt;0,0,(N67-50))), "" )</f>
         <v/>
       </c>
       <c r="K67">
         <v>1</v>
       </c>
       <c r="N67">
-        <f t="shared" ref="N67:N130" si="9">IF((H67+I67+J67+L67+M67+O67)&lt;70,IF((H67+I67+J67+L67+M67+O67)&gt;59,70,(H67+I67+J67+L67+M67+O67)),(H67+I67+J67+L67+M67+O67))</f>
+        <f t="shared" ref="N67:N90" si="9">IF((H67+I67+J67+L67+M67+O67)&lt;70,IF((H67+I67+J67+L67+M67+O67)&gt;59,70,(H67+I67+J67+L67+M67+O67)),(H67+I67+J67+L67+M67+O67))</f>
         <v>0</v>
       </c>
     </row>
@@ -3603,12 +3684,15 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="I71">
+        <v>10</v>
+      </c>
       <c r="K71">
         <v>1</v>
       </c>
       <c r="N71">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3637,12 +3721,15 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="I72">
+        <v>10</v>
+      </c>
       <c r="K72">
         <v>1</v>
       </c>
       <c r="N72">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3671,12 +3758,15 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="I73">
+        <v>10</v>
+      </c>
       <c r="K73">
         <v>1</v>
       </c>
       <c r="N73">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3705,12 +3795,15 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="I74">
+        <v>10</v>
+      </c>
       <c r="K74">
         <v>1</v>
       </c>
       <c r="N74">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3739,12 +3832,15 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="I75">
+        <v>10</v>
+      </c>
       <c r="K75">
         <v>1</v>
       </c>
       <c r="N75">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3841,12 +3937,15 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="I78">
+        <v>10</v>
+      </c>
       <c r="K78">
         <v>1</v>
       </c>
       <c r="N78">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3909,12 +4008,15 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="I80">
+        <v>10</v>
+      </c>
       <c r="K80">
         <v>1</v>
       </c>
       <c r="N80">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -4011,12 +4113,15 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="I83">
+        <v>10</v>
+      </c>
       <c r="K83">
         <v>1</v>
       </c>
       <c r="N83">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -4079,12 +4184,15 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="I85">
+        <v>10</v>
+      </c>
       <c r="K85">
         <v>1</v>
       </c>
       <c r="N85">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -4113,12 +4221,15 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="I86">
+        <v>10</v>
+      </c>
       <c r="K86">
         <v>1</v>
       </c>
       <c r="N86">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -4181,12 +4292,15 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="I88">
+        <v>10</v>
+      </c>
       <c r="K88">
         <v>1</v>
       </c>
       <c r="N88">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -4249,2208 +4363,15 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="I90">
+        <v>10</v>
+      </c>
       <c r="K90">
         <v>1</v>
       </c>
       <c r="N90">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="7"/>
-      <c r="B91" s="8"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E91" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F91" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G91" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K91">
-        <v>1</v>
-      </c>
-      <c r="N91">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="7"/>
-      <c r="B92" s="8"/>
-      <c r="C92" s="8"/>
-      <c r="D92" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E92" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F92" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G92" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K92">
-        <v>1</v>
-      </c>
-      <c r="N92">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="7"/>
-      <c r="B93" s="8"/>
-      <c r="C93" s="8"/>
-      <c r="D93" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E93" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F93" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G93" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K93">
-        <v>1</v>
-      </c>
-      <c r="N93">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="7"/>
-      <c r="B94" s="8"/>
-      <c r="C94" s="8"/>
-      <c r="D94" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E94" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F94" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G94" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K94">
-        <v>1</v>
-      </c>
-      <c r="N94">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="7"/>
-      <c r="B95" s="8"/>
-      <c r="C95" s="8"/>
-      <c r="D95" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E95" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F95" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G95" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K95">
-        <v>1</v>
-      </c>
-      <c r="N95">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="7"/>
-      <c r="B96" s="8"/>
-      <c r="C96" s="8"/>
-      <c r="D96" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E96" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F96" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G96" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K96">
-        <v>1</v>
-      </c>
-      <c r="N96">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="7"/>
-      <c r="B97" s="8"/>
-      <c r="C97" s="8"/>
-      <c r="D97" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E97" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F97" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G97" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K97">
-        <v>1</v>
-      </c>
-      <c r="N97">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="7"/>
-      <c r="B98" s="8"/>
-      <c r="C98" s="8"/>
-      <c r="D98" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E98" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F98" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G98" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K98">
-        <v>1</v>
-      </c>
-      <c r="N98">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="7"/>
-      <c r="B99" s="8"/>
-      <c r="C99" s="8"/>
-      <c r="D99" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E99" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F99" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G99" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K99">
-        <v>1</v>
-      </c>
-      <c r="N99">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="7"/>
-      <c r="B100" s="8"/>
-      <c r="C100" s="8"/>
-      <c r="D100" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E100" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F100" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G100" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K100">
-        <v>1</v>
-      </c>
-      <c r="N100">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="7"/>
-      <c r="B101" s="8"/>
-      <c r="C101" s="8"/>
-      <c r="D101" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E101" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F101" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G101" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K101">
-        <v>1</v>
-      </c>
-      <c r="N101">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="7"/>
-      <c r="B102" s="8"/>
-      <c r="C102" s="8"/>
-      <c r="D102" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E102" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F102" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G102" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K102">
-        <v>1</v>
-      </c>
-      <c r="N102">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="7"/>
-      <c r="B103" s="8"/>
-      <c r="C103" s="8"/>
-      <c r="D103" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E103" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F103" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G103" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K103">
-        <v>1</v>
-      </c>
-      <c r="N103">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="7"/>
-      <c r="B104" s="8"/>
-      <c r="C104" s="8"/>
-      <c r="D104" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E104" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F104" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G104" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K104">
-        <v>1</v>
-      </c>
-      <c r="N104">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="7"/>
-      <c r="B105" s="8"/>
-      <c r="C105" s="8"/>
-      <c r="D105" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E105" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F105" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G105" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K105">
-        <v>1</v>
-      </c>
-      <c r="N105">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="7"/>
-      <c r="B106" s="8"/>
-      <c r="C106" s="8"/>
-      <c r="D106" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E106" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F106" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G106" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K106">
-        <v>1</v>
-      </c>
-      <c r="N106">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="7"/>
-      <c r="B107" s="8"/>
-      <c r="C107" s="8"/>
-      <c r="D107" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E107" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F107" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G107" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K107">
-        <v>1</v>
-      </c>
-      <c r="N107">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="7"/>
-      <c r="B108" s="8"/>
-      <c r="C108" s="8"/>
-      <c r="D108" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E108" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F108" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G108" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K108">
-        <v>1</v>
-      </c>
-      <c r="N108">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="7"/>
-      <c r="B109" s="8"/>
-      <c r="C109" s="8"/>
-      <c r="D109" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E109" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F109" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G109" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K109">
-        <v>1</v>
-      </c>
-      <c r="N109">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="7"/>
-      <c r="B110" s="8"/>
-      <c r="C110" s="8"/>
-      <c r="D110" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E110" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F110" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G110" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K110">
-        <v>1</v>
-      </c>
-      <c r="N110">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="7"/>
-      <c r="B111" s="8"/>
-      <c r="C111" s="8"/>
-      <c r="D111" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E111" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F111" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G111" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K111">
-        <v>1</v>
-      </c>
-      <c r="N111">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="7"/>
-      <c r="B112" s="8"/>
-      <c r="C112" s="8"/>
-      <c r="D112" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E112" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F112" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G112" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K112">
-        <v>1</v>
-      </c>
-      <c r="N112">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="7"/>
-      <c r="B113" s="8"/>
-      <c r="C113" s="8"/>
-      <c r="D113" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E113" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F113" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G113" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K113">
-        <v>1</v>
-      </c>
-      <c r="N113">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="7"/>
-      <c r="B114" s="8"/>
-      <c r="C114" s="8"/>
-      <c r="D114" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E114" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F114" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G114" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K114">
-        <v>1</v>
-      </c>
-      <c r="N114">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="7"/>
-      <c r="B115" s="8"/>
-      <c r="C115" s="8"/>
-      <c r="D115" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E115" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F115" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G115" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K115">
-        <v>1</v>
-      </c>
-      <c r="N115">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="7"/>
-      <c r="B116" s="8"/>
-      <c r="C116" s="8"/>
-      <c r="D116" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E116" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F116" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G116" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K116">
-        <v>1</v>
-      </c>
-      <c r="N116">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="7"/>
-      <c r="B117" s="8"/>
-      <c r="C117" s="8"/>
-      <c r="D117" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E117" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F117" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G117" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K117">
-        <v>1</v>
-      </c>
-      <c r="N117">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="7"/>
-      <c r="B118" s="8"/>
-      <c r="C118" s="8"/>
-      <c r="D118" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E118" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F118" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G118" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="K118">
-        <v>1</v>
-      </c>
-      <c r="N118">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="7"/>
-      <c r="B119" s="8"/>
-      <c r="C119" s="8"/>
-      <c r="D119" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E119" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F119" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G119" s="6" t="str">
-        <f t="shared" ref="G67:G130" si="10">IF((N119)&gt;=70,IF((N119-50)&gt;50,50,IF((N119-50)&lt;0,0,(N119-50))), "" )</f>
-        <v/>
-      </c>
-      <c r="K119">
-        <v>1</v>
-      </c>
-      <c r="N119">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="7"/>
-      <c r="B120" s="8"/>
-      <c r="C120" s="8"/>
-      <c r="D120" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E120" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F120" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G120" s="6" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="K120">
-        <v>1</v>
-      </c>
-      <c r="N120">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D121" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E121" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F121" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G121" s="6" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="N121">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D122" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E122" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F122" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G122" s="6" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="N122">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D123" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E123" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F123" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G123" s="6" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="N123">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D124" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E124" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F124" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G124" s="6" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="N124">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D125" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E125" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F125" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G125" s="6" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="N125">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D126" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E126" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F126" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G126" s="6" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="N126">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D127" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E127" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F127" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G127" s="6" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="N127">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D128" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E128" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F128" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G128" s="6" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="N128">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D129" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E129" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F129" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G129" s="6" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="N129">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D130" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E130" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F130" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G130" s="6" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="N130">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D131" s="6" t="str">
-        <f t="shared" ref="D131:D164" si="11">IF((N131)&gt;=70,10,"")</f>
-        <v/>
-      </c>
-      <c r="E131" s="2" t="str">
-        <f t="shared" ref="E131:E146" si="12">IF((N131)&gt;=70,20,"")</f>
-        <v/>
-      </c>
-      <c r="F131" s="2" t="str">
-        <f t="shared" ref="F131:F132" si="13">IF((N131)&gt;=70,20,"")</f>
-        <v/>
-      </c>
-      <c r="G131" s="6" t="str">
-        <f t="shared" ref="G131:G147" si="14">IF((N131)&gt;=70,IF((N131-50)&gt;50,50,IF((N131-50)&lt;0,0,(N131-50))), "" )</f>
-        <v/>
-      </c>
-      <c r="N131">
-        <f t="shared" ref="N131:N144" si="15">IF((H131+I131+J131+L131+M131+O131)&lt;70,IF((H131+I131+J131+L131+M131+O131)&gt;59,70,(H131+I131+J131+L131+M131+O131)),(H131+I131+J131+L131+M131+O131))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D132" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E132" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="F132" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="G132" s="6" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="N132">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D133" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E133" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="F133" s="2" t="str">
-        <f t="shared" ref="F131:F190" si="16">IF((N133)&gt;=70,20,"")</f>
-        <v/>
-      </c>
-      <c r="G133" s="6" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="N133">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D134" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E134" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="F134" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G134" s="6" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="N134">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D135" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E135" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="F135" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G135" s="6" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="N135">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D136" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E136" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="F136" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G136" s="6" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="N136">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D137" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E137" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="F137" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G137" s="6" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="N137">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D138" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E138" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="F138" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G138" s="6" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="N138">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D139" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E139" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="F139" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G139" s="6" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="N139">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D140" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E140" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="F140" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G140" s="6" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="N140">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D141" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E141" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="F141" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G141" s="6" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="N141">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D142" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E142" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="F142" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G142" s="6" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="N142">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D143" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E143" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="F143" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G143" s="6" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="N143">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D144" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E144" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="F144" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G144" s="6" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="N144">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D145" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E145" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="F145" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G145" s="6" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-    </row>
-    <row r="146" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D146" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E146" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="F146" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G146" s="6" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-    </row>
-    <row r="147" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D147" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E147" s="2" t="str">
-        <f t="shared" ref="E131:E190" si="17">IF((N147)&gt;=70,20,"")</f>
-        <v/>
-      </c>
-      <c r="F147" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G147" s="6" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-    </row>
-    <row r="148" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D148" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E148" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F148" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G148" s="6" t="str">
-        <f t="shared" ref="G131:G190" si="18">IF((N148)&gt;=70,IF((N148-50)&gt;50,50,IF((N148-50)&lt;0,0,(N148-50))), "" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="149" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D149" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E149" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F149" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G149" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="150" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D150" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E150" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F150" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G150" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="151" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D151" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E151" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F151" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G151" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="152" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D152" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E152" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F152" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G152" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="153" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D153" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E153" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F153" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G153" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="154" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D154" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E154" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F154" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G154" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="155" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D155" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E155" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F155" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G155" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="156" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D156" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E156" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F156" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G156" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="157" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D157" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E157" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F157" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G157" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="158" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D158" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E158" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F158" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G158" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="159" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D159" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E159" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F159" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G159" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="160" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D160" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E160" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F160" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G160" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="161" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D161" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E161" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F161" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G161" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="162" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D162" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E162" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F162" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G162" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="163" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D163" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E163" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F163" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G163" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="164" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D164" s="6" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="E164" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F164" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G164" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="165" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D165" s="6" t="str">
-        <f t="shared" ref="D131:D190" si="19">IF((N165)&gt;=70,10,"")</f>
-        <v/>
-      </c>
-      <c r="E165" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F165" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G165" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="166" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D166" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E166" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F166" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G166" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="167" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D167" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E167" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F167" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G167" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="168" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D168" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E168" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F168" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G168" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="169" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D169" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E169" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F169" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G169" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="170" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D170" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E170" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F170" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G170" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="171" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D171" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E171" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F171" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G171" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="172" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D172" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E172" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F172" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G172" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="173" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D173" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E173" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F173" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G173" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="174" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D174" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E174" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F174" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G174" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="175" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D175" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E175" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F175" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G175" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="176" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D176" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E176" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F176" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G176" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="177" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D177" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E177" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F177" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G177" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="178" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D178" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E178" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F178" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G178" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="179" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D179" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E179" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F179" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G179" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="180" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D180" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E180" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F180" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G180" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="181" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D181" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E181" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F181" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G181" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="182" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D182" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E182" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F182" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G182" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="183" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D183" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E183" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F183" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G183" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="184" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D184" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E184" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F184" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G184" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="185" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D185" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E185" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F185" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G185" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="186" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D186" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E186" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F186" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G186" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="187" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D187" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E187" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F187" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G187" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="188" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D188" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E188" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F188" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G188" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="189" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D189" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E189" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F189" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G189" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-    </row>
-    <row r="190" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D190" s="6" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="E190" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="F190" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G190" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v/>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>